<commit_message>
COHORT 8, DAMS INFO, ECHOMRI EDITION 10/7
</commit_message>
<xml_diff>
--- a/data/echoMRI/Kotz10072025.xlsx
+++ b/data/echoMRI/Kotz10072025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcaballero/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C8D37F-3C52-5540-97E9-AA1596982E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB38DD3-D3DD-B44B-84F8-5ABC3571D494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>RecNumber</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>9362</t>
-  </si>
-  <si>
-    <t>9272</t>
   </si>
   <si>
     <t>9369</t>
@@ -627,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -688,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -717,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -746,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -775,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -804,7 +801,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -833,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -862,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -891,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -920,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -949,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -978,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1007,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1036,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1065,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1094,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1107,8 +1104,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>25</v>
+      <c r="B17">
+        <v>9372</v>
       </c>
       <c r="C17">
         <v>4.24</v>
@@ -1123,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1137,7 +1134,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>5.19</v>
@@ -1152,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1166,7 +1163,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>1.38</v>
@@ -1181,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1195,7 +1192,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>13.14</v>
@@ -1210,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1224,7 +1221,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>1.67</v>
@@ -1239,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1253,7 +1250,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>13.59</v>
@@ -1268,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1282,7 +1279,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>7.24</v>
@@ -1297,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1311,7 +1308,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>6.32</v>
@@ -1326,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1340,7 +1337,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>9.07</v>
@@ -1355,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1369,7 +1366,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>10.23</v>
@@ -1384,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1398,7 +1395,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>7.15</v>
@@ -1413,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1427,7 +1424,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28">
         <v>24.43</v>
@@ -1442,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1456,7 +1453,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>5.7</v>
@@ -1471,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1485,7 +1482,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30">
         <v>2.4500000000000002</v>
@@ -1500,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1514,7 +1511,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31">
         <v>14.87</v>
@@ -1529,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1543,7 +1540,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32">
         <v>4.45</v>
@@ -1558,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -1572,7 +1569,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33">
         <v>2.5299999999999998</v>
@@ -1587,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -1601,7 +1598,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>14.51</v>
@@ -1616,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1630,7 +1627,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35">
         <v>2.33</v>
@@ -1645,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -1659,7 +1656,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>9.73</v>
@@ -1674,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -1688,7 +1685,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37">
         <v>7.33</v>
@@ -1703,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -1717,7 +1714,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>2.09</v>
@@ -1732,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -1746,7 +1743,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>25.63</v>
@@ -1761,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -1775,7 +1772,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40">
         <v>7.6</v>
@@ -1790,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H40">
         <v>1</v>

</xml_diff>